<commit_message>
Finish most API design, except the web pages, and they still needs to be reviewed.
</commit_message>
<xml_diff>
--- a/设计/总体功能列表.xlsx
+++ b/设计/总体功能列表.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\23324\Documents\Codes\Hummingbird\设计\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\HummingBird\设计\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C7AEAD-3497-490B-90F3-0A5AE74B99E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105832AD-473F-4B5E-918B-525196436E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5595" yWindow="0" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="总体需求" sheetId="1" r:id="rId1"/>
+    <sheet name="第一个版本" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
   <si>
     <t>分类</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -195,10 +196,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>按照板块筛选文章</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>保存并跳转到对应的文章页面</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -327,76 +324,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>本地图片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>外源图片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有两种方式添加图片：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过填写URL链接添加</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过“添加本地图片”添加</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图片管理系统用于管理本地图片，他不会去记录任何关于外源图片的信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>博客系统有两种图片类型：</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>本地图片和外源图片</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不过博客系统拥有以下与外源图片相关的功能：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>博客系统会记录每篇文章引用的外源图片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在文章编辑页面中，系统会列出该文章引用的所有外源图片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>博客系统会定期检查这些外源图片是否失效。如果检查到外源图片失效，系统将高亮所有引用了该图片的文章，以让用户处理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一种方式可以用来添加外源图片，也可以用来添加本地图片，但是需要：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 验证URL的内容是否为图片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. 验证URL是否为本地图片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -463,6 +390,9 @@
   <si>
     <t>总体功能列表</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{ count: Number }</t>
   </si>
 </sst>
 </file>
@@ -919,36 +849,36 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.58203125" customWidth="1"/>
-    <col min="2" max="2" width="34.08203125" customWidth="1"/>
+    <col min="1" max="1" width="58.625" customWidth="1"/>
+    <col min="2" max="2" width="34.125" customWidth="1"/>
     <col min="3" max="3" width="43.25" customWidth="1"/>
-    <col min="4" max="4" width="34.58203125" customWidth="1"/>
-    <col min="5" max="5" width="49.58203125" customWidth="1"/>
+    <col min="4" max="4" width="34.625" customWidth="1"/>
+    <col min="5" max="5" width="49.625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:5" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -965,7 +895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
@@ -982,7 +912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -993,13 +923,13 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1007,33 +937,33 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>38</v>
       </c>
@@ -1050,7 +980,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -1061,13 +991,13 @@
         <v>10</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -1075,305 +1005,270 @@
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="E12" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="2" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C20" t="s">
-        <v>81</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1384,4 +1279,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7314880D-7A12-4E43-8E90-A9640C1C456E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>